<commit_message>
added ceil to sums
</commit_message>
<xml_diff>
--- a/out/production/MScanner/file/MScanner.xlsx
+++ b/out/production/MScanner/file/MScanner.xlsx
@@ -2145,60 +2145,60 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="26" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="27" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="1" fillId="27" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2213,16 +2213,12 @@
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2235,162 +2231,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="23" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2497,6 +2337,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="1" fontId="19" fillId="3" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2505,6 +2353,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="1" fontId="19" fillId="3" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2513,6 +2369,14 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2565,140 +2429,372 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="23" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="27" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="27" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="12" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="61" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2757,175 +2853,79 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="12" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="12" fillId="10" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="61" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="26" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
@@ -3345,7 +3345,7 @@
   <dimension ref="A1:BT210"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="C3:H3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3419,10 +3419,10 @@
       <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="201" t="s">
+      <c r="K2" s="237" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="202"/>
+      <c r="L2" s="238"/>
       <c r="M2" s="107" t="s">
         <v>31</v>
       </c>
@@ -3430,18 +3430,18 @@
       <c r="O2" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="195" t="s">
+      <c r="Q2" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="197"/>
-      <c r="W2" s="265" t="s">
+      <c r="R2" s="232"/>
+      <c r="S2" s="232"/>
+      <c r="T2" s="232"/>
+      <c r="U2" s="232"/>
+      <c r="V2" s="233"/>
+      <c r="W2" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="267" t="s">
+      <c r="X2" s="172" t="s">
         <v>25</v>
       </c>
       <c r="Y2" s="105"/>
@@ -3472,26 +3472,26 @@
       <c r="I3" s="104">
         <v>40</v>
       </c>
-      <c r="J3" s="355">
+      <c r="J3" s="160">
         <v>3.2</v>
       </c>
-      <c r="K3" s="203"/>
-      <c r="L3" s="204"/>
+      <c r="K3" s="239"/>
+      <c r="L3" s="240"/>
       <c r="M3" s="109">
-        <v>45188</v>
+        <v>45490</v>
       </c>
       <c r="N3" s="110"/>
       <c r="O3" s="151">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q3" s="198"/>
-      <c r="R3" s="199"/>
-      <c r="S3" s="199"/>
-      <c r="T3" s="199"/>
-      <c r="U3" s="199"/>
-      <c r="V3" s="200"/>
-      <c r="W3" s="266"/>
-      <c r="X3" s="268"/>
+        <v>0.3</v>
+      </c>
+      <c r="Q3" s="234"/>
+      <c r="R3" s="235"/>
+      <c r="S3" s="235"/>
+      <c r="T3" s="235"/>
+      <c r="U3" s="235"/>
+      <c r="V3" s="236"/>
+      <c r="W3" s="178"/>
+      <c r="X3" s="173"/>
       <c r="Y3" s="105"/>
       <c r="Z3" s="111"/>
       <c r="AA3" s="105"/>
@@ -3499,34 +3499,34 @@
     <row r="4" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="211">
+      <c r="C4" s="250">
         <f ca="1">TODAY()</f>
-        <v>45364</v>
-      </c>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="213"/>
-      <c r="I4" s="205">
-        <f>ROUNDUP((SUM(C3:I3)*O3 +SUM(C3:I3) )*J3,0)</f>
-        <v>164</v>
-      </c>
-      <c r="J4" s="208">
-        <f>ROUNDUP((((SUM(D3:F3)+SUM(H3:I3)+(SUM(G3)*0.75))*O3)+(SUM(D3:F3)+SUM(H3:I3)+(SUM(G3)*0.75)))*J3,0)</f>
-        <v>164</v>
+        <v>45490</v>
+      </c>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="252"/>
+      <c r="I4" s="241">
+        <f>ROUNDUP((SUM(C3:I3)*O3 +SUM(C3:I3) )*J3,-1)</f>
+        <v>170</v>
+      </c>
+      <c r="J4" s="244">
+        <f>ROUNDUP((((SUM(D3:F3)+SUM(H3:I3)+(SUM(G3)*0.75))*O3)+(SUM(D3:F3)+SUM(H3:I3)+(SUM(G3)*0.75)))*J3,-1)</f>
+        <v>170</v>
       </c>
       <c r="K4" s="112"/>
       <c r="L4" s="112"/>
       <c r="M4" s="113"/>
       <c r="N4" s="113"/>
       <c r="O4" s="113"/>
-      <c r="Q4" s="186"/>
-      <c r="R4" s="187"/>
-      <c r="S4" s="187"/>
-      <c r="T4" s="187"/>
-      <c r="U4" s="187"/>
-      <c r="V4" s="188"/>
+      <c r="Q4" s="247"/>
+      <c r="R4" s="248"/>
+      <c r="S4" s="248"/>
+      <c r="T4" s="248"/>
+      <c r="U4" s="248"/>
+      <c r="V4" s="249"/>
       <c r="W4" s="114"/>
       <c r="X4" s="115"/>
       <c r="Y4" s="1"/>
@@ -3535,16 +3535,16 @@
     <row r="5" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="214" t="s">
+      <c r="C5" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="215"/>
-      <c r="E5" s="215"/>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215"/>
-      <c r="H5" s="216"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="209"/>
+      <c r="D5" s="254"/>
+      <c r="E5" s="254"/>
+      <c r="F5" s="254"/>
+      <c r="G5" s="254"/>
+      <c r="H5" s="255"/>
+      <c r="I5" s="242"/>
+      <c r="J5" s="245"/>
       <c r="K5" s="112"/>
       <c r="L5" s="112"/>
       <c r="N5" s="116" t="s">
@@ -3567,21 +3567,21 @@
     <row r="6" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="217"/>
-      <c r="D6" s="218"/>
-      <c r="E6" s="218"/>
-      <c r="F6" s="218"/>
-      <c r="G6" s="218"/>
-      <c r="H6" s="219"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="210"/>
+      <c r="C6" s="256"/>
+      <c r="D6" s="257"/>
+      <c r="E6" s="257"/>
+      <c r="F6" s="257"/>
+      <c r="G6" s="257"/>
+      <c r="H6" s="258"/>
+      <c r="I6" s="243"/>
+      <c r="J6" s="246"/>
       <c r="K6" s="112"/>
       <c r="L6" s="112"/>
-      <c r="N6" s="168">
-        <v>0.184</v>
-      </c>
-      <c r="O6" s="220">
-        <v>0.27900000000000003</v>
+      <c r="N6" s="279">
+        <v>0.19989999999999999</v>
+      </c>
+      <c r="O6" s="259">
+        <v>0.19989999999999999</v>
       </c>
       <c r="Q6" s="174"/>
       <c r="R6" s="175"/>
@@ -3607,8 +3607,8 @@
       <c r="J7" s="103"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-      <c r="N7" s="169"/>
-      <c r="O7" s="221"/>
+      <c r="N7" s="280"/>
+      <c r="O7" s="260"/>
       <c r="Q7" s="174"/>
       <c r="R7" s="175"/>
       <c r="S7" s="175"/>
@@ -3624,24 +3624,24 @@
     <row r="8" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="234" t="s">
+      <c r="C8" s="194" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="235"/>
-      <c r="E8" s="236"/>
-      <c r="F8" s="193" t="s">
+      <c r="D8" s="195"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="212" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="193" t="s">
+      <c r="G8" s="212" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="240" t="s">
+      <c r="H8" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="241"/>
-      <c r="J8" s="241"/>
-      <c r="K8" s="241"/>
-      <c r="L8" s="242"/>
+      <c r="I8" s="201"/>
+      <c r="J8" s="201"/>
+      <c r="K8" s="201"/>
+      <c r="L8" s="202"/>
       <c r="M8" s="121"/>
       <c r="N8" s="122" t="s">
         <v>36</v>
@@ -3664,29 +3664,29 @@
     <row r="9" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="237"/>
-      <c r="D9" s="238"/>
-      <c r="E9" s="239"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="243"/>
-      <c r="I9" s="244"/>
-      <c r="J9" s="244"/>
-      <c r="K9" s="244"/>
-      <c r="L9" s="245"/>
+      <c r="C9" s="197"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="203"/>
+      <c r="I9" s="204"/>
+      <c r="J9" s="204"/>
+      <c r="K9" s="204"/>
+      <c r="L9" s="205"/>
       <c r="M9" s="121"/>
-      <c r="N9" s="232">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="O9" s="232">
-        <v>0.22</v>
-      </c>
-      <c r="Q9" s="183"/>
-      <c r="R9" s="184"/>
-      <c r="S9" s="184"/>
-      <c r="T9" s="184"/>
-      <c r="U9" s="184"/>
-      <c r="V9" s="185"/>
+      <c r="N9" s="192">
+        <v>0.17</v>
+      </c>
+      <c r="O9" s="192">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="Q9" s="261"/>
+      <c r="R9" s="262"/>
+      <c r="S9" s="262"/>
+      <c r="T9" s="262"/>
+      <c r="U9" s="262"/>
+      <c r="V9" s="263"/>
       <c r="W9" s="118"/>
       <c r="X9" s="119"/>
       <c r="Y9" s="105"/>
@@ -3705,22 +3705,22 @@
       <c r="E10" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
+      <c r="F10" s="213"/>
+      <c r="G10" s="213"/>
       <c r="H10" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="246" t="s">
+      <c r="I10" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="247"/>
-      <c r="K10" s="189" t="s">
+      <c r="J10" s="207"/>
+      <c r="K10" s="264" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="190"/>
+      <c r="L10" s="265"/>
       <c r="M10" s="121"/>
-      <c r="N10" s="233"/>
-      <c r="O10" s="233"/>
+      <c r="N10" s="193"/>
+      <c r="O10" s="193"/>
       <c r="Q10" s="174"/>
       <c r="R10" s="175"/>
       <c r="S10" s="175"/>
@@ -3740,34 +3740,34 @@
         <v>38</v>
       </c>
       <c r="D11" s="124">
-        <f>ROUNDUP($N$20*1.016,0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20*1.016,-1)</f>
+        <v>180</v>
       </c>
       <c r="E11" s="125">
-        <f>ROUNDUP($O$20*1.016,0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20*1.016,-1)</f>
+        <v>180</v>
       </c>
       <c r="F11" s="65">
         <f>ROUNDUP(PMT($N$9/12,3,-D11),0)</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G11" s="77">
         <f>ROUNDUP(PMT($N$9/12,3,-E11),0)</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H11" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="250">
+      <c r="I11" s="214">
         <f>ROUNDUP(PMT($O$9/12,6,-$N$20),0)</f>
-        <v>30</v>
-      </c>
-      <c r="J11" s="251"/>
-      <c r="K11" s="172">
+        <v>31</v>
+      </c>
+      <c r="J11" s="215"/>
+      <c r="K11" s="208">
         <f>ROUNDUP(PMT($O$9/12,6,-$O$20),0)</f>
-        <v>30</v>
-      </c>
-      <c r="L11" s="173"/>
+        <v>31</v>
+      </c>
+      <c r="L11" s="209"/>
       <c r="M11" s="121"/>
       <c r="N11" s="126" t="s">
         <v>54</v>
@@ -3795,37 +3795,37 @@
         <v>9</v>
       </c>
       <c r="D12" s="124">
-        <f>ROUNDUP($N$20*1.021,0)</f>
-        <v>168</v>
+        <f>ROUNDUP($N$20*1.021,-1)</f>
+        <v>180</v>
       </c>
       <c r="E12" s="125">
-        <f>ROUNDUP($O$20*1.021,0)</f>
-        <v>168</v>
+        <f>ROUNDUP($O$20*1.021,-1)</f>
+        <v>180</v>
       </c>
       <c r="F12" s="67">
         <f>ROUNDUP(PMT($N$9/12,6,-D12),0)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G12" s="78">
         <f>ROUNDUP(PMT($N$9/12,6,-E12),0)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="170">
+      <c r="I12" s="216">
         <f>ROUNDUP(PMT($O$9/12,12,-$N$20),0)</f>
         <v>16</v>
       </c>
-      <c r="J12" s="171"/>
-      <c r="K12" s="172">
+      <c r="J12" s="217"/>
+      <c r="K12" s="208">
         <f>ROUNDUP(PMT($O$9/12,12,-$O$20),0)</f>
         <v>16</v>
       </c>
-      <c r="L12" s="173"/>
+      <c r="L12" s="209"/>
       <c r="M12" s="121"/>
       <c r="N12" s="125">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="O12" s="124">
         <v>0</v>
@@ -3850,37 +3850,37 @@
         <v>39</v>
       </c>
       <c r="D13" s="124">
-        <f>ROUNDUP($N$20*1.031,0)</f>
-        <v>170</v>
+        <f>ROUNDUP($N$20*1.031,-1)</f>
+        <v>180</v>
       </c>
       <c r="E13" s="125">
-        <f>ROUNDUP($O$20*1.031,0)</f>
-        <v>170</v>
+        <f>ROUNDUP($O$20*1.031,-1)</f>
+        <v>180</v>
       </c>
       <c r="F13" s="67">
         <f>ROUNDUP(PMT($N$9/12,10,-D13),0)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="78">
         <f>ROUNDUP(PMT($N$9/12,10,-E13),0)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="170">
+      <c r="I13" s="216">
         <f>ROUNDUP(PMT($O$9/12,18,-$N$20),0)</f>
-        <v>11</v>
-      </c>
-      <c r="J13" s="171"/>
-      <c r="K13" s="172">
+        <v>12</v>
+      </c>
+      <c r="J13" s="217"/>
+      <c r="K13" s="208">
         <f>ROUNDUP(PMT($O$9/12,18,-$O$20),0)</f>
-        <v>11</v>
-      </c>
-      <c r="L13" s="173"/>
+        <v>12</v>
+      </c>
+      <c r="L13" s="209"/>
       <c r="M13" s="121"/>
       <c r="N13" s="125">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="O13" s="129">
         <v>0</v>
@@ -3905,37 +3905,37 @@
         <v>10</v>
       </c>
       <c r="D14" s="124">
-        <f>ROUNDUP($N$20*1.037,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.037,-1)</f>
+        <v>180</v>
       </c>
       <c r="E14" s="125">
-        <f>ROUNDUP($O$20*1.037,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.037,-1)</f>
+        <v>180</v>
       </c>
       <c r="F14" s="67">
         <f>ROUNDUP(PMT($N$9/12,12,-D14),0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="78">
         <f>ROUNDUP(PMT($N$9/12,12,-E14),0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H14" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="170">
+      <c r="I14" s="216">
         <f>ROUNDUP(PMT($O$9/12,24,-$N$20),0)</f>
         <v>9</v>
       </c>
-      <c r="J14" s="171"/>
-      <c r="K14" s="172">
+      <c r="J14" s="217"/>
+      <c r="K14" s="208">
         <f>ROUNDUP(PMT($O$9/12,24,-$O$20),0)</f>
         <v>9</v>
       </c>
-      <c r="L14" s="173"/>
+      <c r="L14" s="209"/>
       <c r="M14" s="121"/>
       <c r="N14" s="125">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="O14" s="129">
         <v>0</v>
@@ -3960,37 +3960,37 @@
         <v>40</v>
       </c>
       <c r="D15" s="124">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="E15" s="125">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="F15" s="67">
         <f>ROUNDUP(PMT($N$9/12,15,-D15),0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G15" s="78">
         <f>ROUNDUP(PMT($N$9/12,15,-E15),0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="170">
+      <c r="I15" s="216">
         <f>ROUNDUP(PMT($O$9/12,36,-$N$20),0)</f>
         <v>7</v>
       </c>
-      <c r="J15" s="171"/>
-      <c r="K15" s="172">
+      <c r="J15" s="217"/>
+      <c r="K15" s="208">
         <f>ROUNDUP(PMT($O$9/12,36,-$O$20),0)</f>
         <v>7</v>
       </c>
-      <c r="L15" s="173"/>
+      <c r="L15" s="209"/>
       <c r="M15" s="121"/>
       <c r="N15" s="125">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="O15" s="129">
         <v>0</v>
@@ -4015,37 +4015,37 @@
         <v>11</v>
       </c>
       <c r="D16" s="124">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="E16" s="125">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="F16" s="67">
         <f>ROUNDUP(PMT($N$9/12,18,-D16),0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" s="78">
         <f>ROUNDUP(PMT($N$9/12,18,-E16),0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="263">
+      <c r="I16" s="229">
         <f>ROUNDUP(PMT($O$9/12,48,-$N$20),0)</f>
         <v>6</v>
       </c>
-      <c r="J16" s="264"/>
-      <c r="K16" s="248">
+      <c r="J16" s="230"/>
+      <c r="K16" s="210">
         <f>ROUNDUP(PMT($O$9/12,48,-$O$20),0)</f>
         <v>6</v>
       </c>
-      <c r="L16" s="249"/>
+      <c r="L16" s="211"/>
       <c r="M16" s="121"/>
-      <c r="N16" s="132">
-        <v>1.6</v>
+      <c r="N16" s="125">
+        <v>0</v>
       </c>
       <c r="O16" s="129">
         <v>0</v>
@@ -4070,12 +4070,12 @@
         <v>12</v>
       </c>
       <c r="D17" s="124">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="E17" s="125">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="F17" s="67">
         <f>ROUNDUP(PMT($N$9/12,24,-D17),0)</f>
@@ -4085,15 +4085,15 @@
         <f>ROUNDUP(PMT($N$9/12,24,-E17),0)</f>
         <v>9</v>
       </c>
-      <c r="H17" s="258" t="s">
+      <c r="H17" s="224" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="259"/>
-      <c r="J17" s="260"/>
-      <c r="K17" s="193" t="s">
+      <c r="I17" s="225"/>
+      <c r="J17" s="226"/>
+      <c r="K17" s="212" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="193" t="s">
+      <c r="L17" s="212" t="s">
         <v>16</v>
       </c>
       <c r="M17" s="121"/>
@@ -4121,12 +4121,12 @@
         <v>13</v>
       </c>
       <c r="D18" s="124">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="E18" s="125">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="F18" s="67">
         <f>ROUNDUP(PMT($N$9/12,36,-D18),0)</f>
@@ -4145,13 +4145,13 @@
       <c r="J18" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="194"/>
-      <c r="L18" s="194"/>
+      <c r="K18" s="213"/>
+      <c r="L18" s="213"/>
       <c r="M18" s="121"/>
-      <c r="N18" s="230" t="s">
+      <c r="N18" s="190" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="231"/>
+      <c r="O18" s="191"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="174"/>
       <c r="R18" s="175"/>
@@ -4170,39 +4170,39 @@
         <v>32</v>
       </c>
       <c r="D19" s="134">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="E19" s="132">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="F19" s="83">
         <f>ROUNDUP(PMT($N$9/12,48,-D19),0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G19" s="84">
         <f>ROUNDUP(PMT($N$9/12,48,-E19),0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="91">
-        <f>ROUNDUP($N$20/100*(100+O22),0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20/100*(100+O22),-1)</f>
+        <v>180</v>
       </c>
       <c r="J19" s="91">
-        <f>ROUNDUP($O$20/100*(100+O22),0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20/100*(100+O22),-1)</f>
+        <v>180</v>
       </c>
       <c r="K19" s="125">
         <f>ROUNDUP(I19/4,0)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L19" s="137">
         <f>ROUNDUP(J19/4,0)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M19" s="121"/>
       <c r="N19" s="85" t="s">
@@ -4225,44 +4225,44 @@
     <row r="20" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="255" t="s">
+      <c r="C20" s="221" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="256"/>
-      <c r="E20" s="257"/>
-      <c r="F20" s="261" t="s">
+      <c r="D20" s="222"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="261" t="s">
+      <c r="G20" s="227" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="68" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="71">
-        <f>ROUNDUP($N$20/100*(100+O23),0)</f>
-        <v>173</v>
+        <f>ROUNDUP($N$20/100*(100+O23),-1)</f>
+        <v>180</v>
       </c>
       <c r="J20" s="71">
-        <f>ROUNDUP($O$20/100*(100+O23),0)</f>
-        <v>173</v>
+        <f>ROUNDUP($O$20/100*(100+O23),-1)</f>
+        <v>180</v>
       </c>
       <c r="K20" s="138">
         <f>ROUNDUP(I20/5,0)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L20" s="133">
         <f>ROUNDUP(J20/5,0)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M20" s="121"/>
       <c r="N20" s="86">
         <f>I4-E37</f>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="O20" s="86">
         <f>J4-E37</f>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="174"/>
@@ -4287,17 +4287,17 @@
       <c r="E21" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="262"/>
-      <c r="G21" s="262"/>
-      <c r="H21" s="252" t="s">
+      <c r="F21" s="228"/>
+      <c r="G21" s="228"/>
+      <c r="H21" s="218" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="253"/>
-      <c r="J21" s="254"/>
-      <c r="K21" s="191" t="s">
+      <c r="I21" s="219"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="266" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="191" t="s">
+      <c r="L21" s="266" t="s">
         <v>16</v>
       </c>
       <c r="M21" s="121"/>
@@ -4325,20 +4325,20 @@
         <v>9</v>
       </c>
       <c r="D22" s="91">
-        <f>ROUNDUP($N$20/100*(100+N12),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20/100*(100+N12),-1)</f>
+        <v>170</v>
       </c>
       <c r="E22" s="91">
-        <f>ROUNDUP($O$20/100*(100+N12),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20/100*(100+N12),-1)</f>
+        <v>170</v>
       </c>
       <c r="F22" s="72" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,6,-D22),0)</f>
-        <v>~30</v>
+        <v>~31</v>
       </c>
       <c r="G22" s="72" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,6,-E22),0)</f>
-        <v>~30</v>
+        <v>~31</v>
       </c>
       <c r="H22" s="99" t="s">
         <v>7</v>
@@ -4349,10 +4349,10 @@
       <c r="J22" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="192"/>
-      <c r="L22" s="192"/>
+      <c r="K22" s="267"/>
+      <c r="L22" s="267"/>
       <c r="M22" s="121"/>
-      <c r="N22" s="274">
+      <c r="N22" s="166">
         <v>0.14599999999999999</v>
       </c>
       <c r="O22" s="124">
@@ -4376,12 +4376,12 @@
         <v>10</v>
       </c>
       <c r="D23" s="70">
-        <f>ROUNDUP($N$20/100*(100+N13),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20/100*(100+N13),-1)</f>
+        <v>170</v>
       </c>
       <c r="E23" s="70">
-        <f>ROUNDUP($O$20/100*(100+N13),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20/100*(100+N13),-1)</f>
+        <v>170</v>
       </c>
       <c r="F23" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,12,-D23),0)</f>
@@ -4395,23 +4395,23 @@
         <v>9</v>
       </c>
       <c r="I23" s="91">
-        <f t="shared" ref="I23:I28" si="0">ROUNDUP($N$20/100*(100+O12),0)</f>
-        <v>164</v>
+        <f t="shared" ref="I23:I28" si="0">ROUNDUP($N$20/100*(100+O12),-1)</f>
+        <v>170</v>
       </c>
       <c r="J23" s="91">
-        <f t="shared" ref="J23:J28" si="1">ROUNDUP($O$20/100*(100+O12),0)</f>
-        <v>164</v>
+        <f t="shared" ref="J23:J28" si="1">ROUNDUP($O$20/100*(100+O12),-1)</f>
+        <v>170</v>
       </c>
       <c r="K23" s="72" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,6,-I23),0)</f>
-        <v>~30</v>
+        <v>~31</v>
       </c>
       <c r="L23" s="72" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,6,-J23),0)</f>
-        <v>~30</v>
+        <v>~31</v>
       </c>
       <c r="M23" s="121"/>
-      <c r="N23" s="275"/>
+      <c r="N23" s="167"/>
       <c r="O23" s="133">
         <v>5.3</v>
       </c>
@@ -4433,31 +4433,31 @@
         <v>11</v>
       </c>
       <c r="D24" s="70">
-        <f>ROUNDUP($N$20/100*(100+N14),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20/100*(100+N14),-1)</f>
+        <v>170</v>
       </c>
       <c r="E24" s="70">
-        <f>ROUNDUP($O$20/100*(100+N14),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20/100*(100+N14),-1)</f>
+        <v>170</v>
       </c>
       <c r="F24" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,18,-D24),0)</f>
-        <v>~11</v>
+        <v>~12</v>
       </c>
       <c r="G24" s="79" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,18,-E24),0)</f>
-        <v>~11</v>
+        <v>~12</v>
       </c>
       <c r="H24" s="69" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="70">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J24" s="70">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K24" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,12,-I24),0)</f>
@@ -4471,12 +4471,12 @@
       <c r="N24" s="94"/>
       <c r="O24" s="121"/>
       <c r="P24" s="136"/>
-      <c r="Q24" s="183"/>
-      <c r="R24" s="184"/>
-      <c r="S24" s="184"/>
-      <c r="T24" s="184"/>
-      <c r="U24" s="184"/>
-      <c r="V24" s="185"/>
+      <c r="Q24" s="261"/>
+      <c r="R24" s="262"/>
+      <c r="S24" s="262"/>
+      <c r="T24" s="262"/>
+      <c r="U24" s="262"/>
+      <c r="V24" s="263"/>
       <c r="W24" s="118"/>
       <c r="X24" s="119"/>
       <c r="Z24" s="105"/>
@@ -4488,12 +4488,12 @@
         <v>12</v>
       </c>
       <c r="D25" s="70">
-        <f>ROUNDUP($N$20/100*(100+N15),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20/100*(100+N15),-1)</f>
+        <v>170</v>
       </c>
       <c r="E25" s="70">
-        <f>ROUNDUP($O$20/100*(100+N15),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20/100*(100+N15),-1)</f>
+        <v>170</v>
       </c>
       <c r="F25" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,24,-D25),0)</f>
@@ -4508,11 +4508,11 @@
       </c>
       <c r="I25" s="70">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J25" s="70">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K25" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,18,-I25),0)</f>
@@ -4542,12 +4542,12 @@
         <v>13</v>
       </c>
       <c r="D26" s="70">
-        <f>ROUNDUP($N$20/100*(100+N16),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($N$20/100*(100+N16),-1)</f>
+        <v>170</v>
       </c>
       <c r="E26" s="70">
-        <f>ROUNDUP($O$20/100*(100+N16),0)</f>
-        <v>167</v>
+        <f>ROUNDUP($O$20/100*(100+N16),-1)</f>
+        <v>170</v>
       </c>
       <c r="F26" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($N$6/12,36,-D26),0)</f>
@@ -4562,11 +4562,11 @@
       </c>
       <c r="I26" s="70">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J26" s="70">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K26" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,24,-I26),0)</f>
@@ -4592,23 +4592,23 @@
     <row r="27" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="269" t="s">
+      <c r="C27" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="270"/>
-      <c r="E27" s="270"/>
-      <c r="F27" s="270"/>
-      <c r="G27" s="271"/>
+      <c r="D27" s="162"/>
+      <c r="E27" s="162"/>
+      <c r="F27" s="162"/>
+      <c r="G27" s="163"/>
       <c r="H27" s="69" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="70">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J27" s="70">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K27" s="73" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,36,-I27),0)</f>
@@ -4637,32 +4637,32 @@
       <c r="C28" s="148" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="278" t="s">
+      <c r="D28" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="279"/>
-      <c r="F28" s="278" t="s">
+      <c r="E28" s="171"/>
+      <c r="F28" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="279"/>
+      <c r="G28" s="171"/>
       <c r="H28" s="75" t="s">
         <v>43</v>
       </c>
       <c r="I28" s="71">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J28" s="71">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K28" s="74" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,60,-I28),0)</f>
-        <v>~6</v>
+        <v>~5</v>
       </c>
       <c r="L28" s="74" t="str">
         <f>"~"&amp;ROUNDUP(PMT($O$6/12,60,-J28),0)</f>
-        <v>~6</v>
+        <v>~5</v>
       </c>
       <c r="M28" s="121"/>
       <c r="N28" s="121"/>
@@ -4683,25 +4683,25 @@
       <c r="C29" s="146" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="276">
+      <c r="D29" s="168">
         <f>ROUNDUP(PMT($N$22/12,13,-$N$20),0)</f>
-        <v>14</v>
-      </c>
-      <c r="E29" s="277"/>
-      <c r="F29" s="276">
+        <v>15</v>
+      </c>
+      <c r="E29" s="169"/>
+      <c r="F29" s="168">
         <f>ROUNDUP(PMT($N$22/12,13,-$O$20),0)</f>
-        <v>14</v>
-      </c>
-      <c r="G29" s="277"/>
-      <c r="H29" s="269" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="169"/>
+      <c r="H29" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="I29" s="270"/>
-      <c r="J29" s="271"/>
-      <c r="K29" s="272" t="s">
+      <c r="I29" s="162"/>
+      <c r="J29" s="163"/>
+      <c r="K29" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="L29" s="272" t="s">
+      <c r="L29" s="164" t="s">
         <v>16</v>
       </c>
       <c r="M29" s="139"/>
@@ -4724,16 +4724,16 @@
       <c r="C30" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="276">
+      <c r="D30" s="168">
         <f>ROUNDUP(PMT($N$22/12,15,-$N$20),0)</f>
         <v>13</v>
       </c>
-      <c r="E30" s="277"/>
-      <c r="F30" s="276">
+      <c r="E30" s="169"/>
+      <c r="F30" s="168">
         <f>ROUNDUP(PMT($N$22/12,15,-$O$20),0)</f>
         <v>13</v>
       </c>
-      <c r="G30" s="277"/>
+      <c r="G30" s="169"/>
       <c r="H30" s="157" t="s">
         <v>7</v>
       </c>
@@ -4743,8 +4743,8 @@
       <c r="J30" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="273"/>
-      <c r="L30" s="273"/>
+      <c r="K30" s="165"/>
+      <c r="L30" s="165"/>
       <c r="M30" s="139"/>
       <c r="N30" s="139"/>
       <c r="O30" s="139"/>
@@ -4765,26 +4765,26 @@
       <c r="C31" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="276">
+      <c r="D31" s="168">
         <f>ROUNDUP(PMT($N$22/12,18,-$N$20),0)</f>
         <v>11</v>
       </c>
-      <c r="E31" s="277"/>
-      <c r="F31" s="276">
+      <c r="E31" s="169"/>
+      <c r="F31" s="168">
         <f>ROUNDUP(PMT($N$22/12,18,-$O$20),0)</f>
         <v>11</v>
       </c>
-      <c r="G31" s="277"/>
+      <c r="G31" s="169"/>
       <c r="H31" s="155" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="154">
-        <f>ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="J31" s="154">
-        <f>ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="K31" s="156" t="str">
         <f>"&lt; "&amp;ROUNDUP(PMT($N$22/12,24,-I31),0)</f>
@@ -4814,34 +4814,34 @@
       <c r="C32" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="276">
+      <c r="D32" s="168">
         <f>ROUNDUP(PMT($N$22/12,24,-$N$20),0)</f>
-        <v>8</v>
-      </c>
-      <c r="E32" s="277"/>
-      <c r="F32" s="276">
+        <v>9</v>
+      </c>
+      <c r="E32" s="169"/>
+      <c r="F32" s="168">
         <f>ROUNDUP(PMT($N$22/12,24,-$O$20),0)</f>
-        <v>8</v>
-      </c>
-      <c r="G32" s="277"/>
+        <v>9</v>
+      </c>
+      <c r="G32" s="169"/>
       <c r="H32" s="152" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="154">
-        <f t="shared" ref="I32:I34" si="2">ROUNDUP($N$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="J32" s="154">
-        <f t="shared" ref="J32:J34" si="3">ROUNDUP($O$20*1.042,0)</f>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="K32" s="156" t="str">
         <f>"&lt; "&amp;ROUNDUP(PMT($N$22/12,36,-I32),0)</f>
-        <v>&lt; 6</v>
+        <v>&lt; 7</v>
       </c>
       <c r="L32" s="156" t="str">
         <f>"&lt; "&amp;ROUNDUP(PMT($N$22/12,36,-J32),0)</f>
-        <v>&lt; 6</v>
+        <v>&lt; 7</v>
       </c>
       <c r="M32" s="139"/>
       <c r="N32" s="139"/>
@@ -4863,26 +4863,26 @@
       <c r="C33" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="276">
+      <c r="D33" s="168">
         <f>ROUNDUP(PMT($N$22/12,36,-$N$20),0)</f>
         <v>6</v>
       </c>
-      <c r="E33" s="277"/>
-      <c r="F33" s="276">
+      <c r="E33" s="169"/>
+      <c r="F33" s="168">
         <f>ROUNDUP(PMT($N$22/12,36,-$O$20),0)</f>
         <v>6</v>
       </c>
-      <c r="G33" s="277"/>
+      <c r="G33" s="169"/>
       <c r="H33" s="152" t="s">
         <v>32</v>
       </c>
       <c r="I33" s="154">
-        <f t="shared" si="2"/>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="J33" s="154">
-        <f t="shared" si="3"/>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="K33" s="156" t="str">
         <f>"&lt; "&amp;ROUNDUP(PMT($N$22/12,48,-I33),0)</f>
@@ -4912,26 +4912,26 @@
       <c r="C34" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="276">
+      <c r="D34" s="168">
         <f>ROUNDUP(PMT($N$22/12,48,-$N$20),0)</f>
         <v>5</v>
       </c>
-      <c r="E34" s="277"/>
-      <c r="F34" s="276">
+      <c r="E34" s="169"/>
+      <c r="F34" s="168">
         <f>ROUNDUP(PMT($N$22/12,48,-$O$20),0)</f>
         <v>5</v>
       </c>
-      <c r="G34" s="277"/>
+      <c r="G34" s="169"/>
       <c r="H34" s="153" t="s">
         <v>43</v>
       </c>
       <c r="I34" s="154">
-        <f t="shared" si="2"/>
-        <v>171</v>
+        <f>ROUNDUP($N$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="J34" s="154">
-        <f t="shared" si="3"/>
-        <v>171</v>
+        <f>ROUNDUP($O$20*1.042,-1)</f>
+        <v>180</v>
       </c>
       <c r="K34" s="156" t="str">
         <f>"&lt; "&amp;ROUNDUP(PMT($N$22/12,60,-I34),0)</f>
@@ -4961,16 +4961,16 @@
       <c r="C35" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="276">
+      <c r="D35" s="168">
         <f>ROUNDUP(PMT($N$22/12,60,-$N$20),0)</f>
-        <v>4</v>
-      </c>
-      <c r="E35" s="277"/>
-      <c r="F35" s="276">
+        <v>5</v>
+      </c>
+      <c r="E35" s="169"/>
+      <c r="F35" s="168">
         <f>ROUNDUP(PMT($N$22/12,60,-$O$20),0)</f>
-        <v>4</v>
-      </c>
-      <c r="G35" s="277"/>
+        <v>5</v>
+      </c>
+      <c r="G35" s="169"/>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
@@ -5009,14 +5009,14 @@
     <row r="37" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="222" t="s">
+      <c r="C37" s="182" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="223"/>
-      <c r="E37" s="226">
+      <c r="D37" s="183"/>
+      <c r="E37" s="186">
         <v>0</v>
       </c>
-      <c r="F37" s="227"/>
+      <c r="F37" s="187"/>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
@@ -5034,10 +5034,10 @@
     <row r="38" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="224"/>
-      <c r="D38" s="225"/>
-      <c r="E38" s="228"/>
-      <c r="F38" s="229"/>
+      <c r="C38" s="184"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="188"/>
+      <c r="F38" s="189"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
       <c r="O38" s="12"/>
@@ -5082,15 +5082,15 @@
     <row r="40" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="160" t="s">
+      <c r="C40" s="271" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="161"/>
-      <c r="E40" s="164">
+      <c r="D40" s="272"/>
+      <c r="E40" s="275">
         <f>C3*J3</f>
         <v>0</v>
       </c>
-      <c r="F40" s="165"/>
+      <c r="F40" s="276"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -5113,10 +5113,10 @@
     <row r="41" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
-      <c r="C41" s="162"/>
-      <c r="D41" s="163"/>
-      <c r="E41" s="166"/>
-      <c r="F41" s="167"/>
+      <c r="C41" s="273"/>
+      <c r="D41" s="274"/>
+      <c r="E41" s="277"/>
+      <c r="F41" s="278"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -5291,12 +5291,12 @@
       <c r="X55" s="119"/>
     </row>
     <row r="56" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q56" s="180"/>
-      <c r="R56" s="181"/>
-      <c r="S56" s="181"/>
-      <c r="T56" s="181"/>
-      <c r="U56" s="181"/>
-      <c r="V56" s="182"/>
+      <c r="Q56" s="179"/>
+      <c r="R56" s="180"/>
+      <c r="S56" s="180"/>
+      <c r="T56" s="180"/>
+      <c r="U56" s="180"/>
+      <c r="V56" s="181"/>
       <c r="W56" s="114"/>
       <c r="X56" s="140"/>
     </row>
@@ -5811,12 +5811,12 @@
       <c r="X107" s="119"/>
     </row>
     <row r="108" spans="17:26" x14ac:dyDescent="0.3">
-      <c r="Q108" s="180"/>
-      <c r="R108" s="181"/>
-      <c r="S108" s="181"/>
-      <c r="T108" s="181"/>
-      <c r="U108" s="181"/>
-      <c r="V108" s="182"/>
+      <c r="Q108" s="179"/>
+      <c r="R108" s="180"/>
+      <c r="S108" s="180"/>
+      <c r="T108" s="180"/>
+      <c r="U108" s="180"/>
+      <c r="V108" s="181"/>
       <c r="W108" s="114"/>
       <c r="X108" s="140"/>
     </row>
@@ -5854,12 +5854,12 @@
       <c r="X111" s="119"/>
     </row>
     <row r="112" spans="17:26" x14ac:dyDescent="0.3">
-      <c r="Q112" s="183"/>
-      <c r="R112" s="184"/>
-      <c r="S112" s="184"/>
-      <c r="T112" s="184"/>
-      <c r="U112" s="184"/>
-      <c r="V112" s="185"/>
+      <c r="Q112" s="261"/>
+      <c r="R112" s="262"/>
+      <c r="S112" s="262"/>
+      <c r="T112" s="262"/>
+      <c r="U112" s="262"/>
+      <c r="V112" s="263"/>
       <c r="W112" s="118"/>
       <c r="X112" s="119"/>
     </row>
@@ -6004,12 +6004,12 @@
       <c r="X126" s="119"/>
     </row>
     <row r="127" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q127" s="183"/>
-      <c r="R127" s="184"/>
-      <c r="S127" s="184"/>
-      <c r="T127" s="184"/>
-      <c r="U127" s="184"/>
-      <c r="V127" s="185"/>
+      <c r="Q127" s="261"/>
+      <c r="R127" s="262"/>
+      <c r="S127" s="262"/>
+      <c r="T127" s="262"/>
+      <c r="U127" s="262"/>
+      <c r="V127" s="263"/>
       <c r="W127" s="118"/>
       <c r="X127" s="119"/>
     </row>
@@ -6324,12 +6324,12 @@
       <c r="X158" s="119"/>
     </row>
     <row r="159" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q159" s="180"/>
-      <c r="R159" s="181"/>
-      <c r="S159" s="181"/>
-      <c r="T159" s="181"/>
-      <c r="U159" s="181"/>
-      <c r="V159" s="182"/>
+      <c r="Q159" s="179"/>
+      <c r="R159" s="180"/>
+      <c r="S159" s="180"/>
+      <c r="T159" s="180"/>
+      <c r="U159" s="180"/>
+      <c r="V159" s="181"/>
       <c r="W159" s="114"/>
       <c r="X159" s="140"/>
     </row>
@@ -6834,12 +6834,12 @@
       <c r="X209" s="119"/>
     </row>
     <row r="210" spans="17:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="Q210" s="177"/>
-      <c r="R210" s="178"/>
-      <c r="S210" s="178"/>
-      <c r="T210" s="178"/>
-      <c r="U210" s="178"/>
-      <c r="V210" s="179"/>
+      <c r="Q210" s="268"/>
+      <c r="R210" s="269"/>
+      <c r="S210" s="269"/>
+      <c r="T210" s="269"/>
+      <c r="U210" s="269"/>
+      <c r="V210" s="270"/>
       <c r="W210" s="141"/>
       <c r="X210" s="142"/>
     </row>
@@ -6849,27 +6849,234 @@
     <protectedRange sqref="Y6 E6:F7 G7 I6:J7" name="Диапазон1_1_2_1"/>
   </protectedRanges>
   <mergeCells count="273">
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="Q207:V207"/>
+    <mergeCell ref="Q208:V208"/>
+    <mergeCell ref="Q209:V209"/>
+    <mergeCell ref="Q175:V175"/>
+    <mergeCell ref="Q176:V176"/>
+    <mergeCell ref="Q177:V177"/>
+    <mergeCell ref="Q178:V178"/>
+    <mergeCell ref="Q179:V179"/>
+    <mergeCell ref="Q197:V197"/>
+    <mergeCell ref="Q180:V180"/>
+    <mergeCell ref="Q181:V181"/>
+    <mergeCell ref="Q191:V191"/>
+    <mergeCell ref="Q192:V192"/>
+    <mergeCell ref="Q193:V193"/>
+    <mergeCell ref="Q194:V194"/>
+    <mergeCell ref="Q195:V195"/>
+    <mergeCell ref="Q196:V196"/>
+    <mergeCell ref="Q166:V166"/>
+    <mergeCell ref="Q174:V174"/>
+    <mergeCell ref="Q165:V165"/>
+    <mergeCell ref="Q182:V182"/>
+    <mergeCell ref="Q190:V190"/>
+    <mergeCell ref="Q167:V167"/>
+    <mergeCell ref="Q168:V168"/>
+    <mergeCell ref="Q169:V169"/>
+    <mergeCell ref="Q170:V170"/>
+    <mergeCell ref="Q171:V171"/>
+    <mergeCell ref="Q172:V172"/>
+    <mergeCell ref="Q173:V173"/>
+    <mergeCell ref="Q189:V189"/>
+    <mergeCell ref="Q183:V183"/>
+    <mergeCell ref="Q184:V184"/>
+    <mergeCell ref="Q185:V185"/>
+    <mergeCell ref="Q186:V186"/>
+    <mergeCell ref="Q187:V187"/>
+    <mergeCell ref="Q188:V188"/>
+    <mergeCell ref="Q210:V210"/>
+    <mergeCell ref="Q198:V198"/>
+    <mergeCell ref="Q199:V199"/>
+    <mergeCell ref="Q200:V200"/>
+    <mergeCell ref="Q201:V201"/>
+    <mergeCell ref="Q202:V202"/>
+    <mergeCell ref="Q203:V203"/>
+    <mergeCell ref="Q204:V204"/>
+    <mergeCell ref="Q205:V205"/>
+    <mergeCell ref="Q206:V206"/>
+    <mergeCell ref="Q164:V164"/>
+    <mergeCell ref="Q147:V147"/>
+    <mergeCell ref="Q155:V155"/>
+    <mergeCell ref="Q156:V156"/>
+    <mergeCell ref="Q148:V148"/>
+    <mergeCell ref="Q149:V149"/>
+    <mergeCell ref="Q150:V150"/>
+    <mergeCell ref="Q151:V151"/>
+    <mergeCell ref="Q152:V152"/>
+    <mergeCell ref="Q153:V153"/>
+    <mergeCell ref="Q154:V154"/>
+    <mergeCell ref="Q163:V163"/>
+    <mergeCell ref="Q157:V157"/>
+    <mergeCell ref="Q158:V158"/>
+    <mergeCell ref="Q159:V159"/>
+    <mergeCell ref="Q160:V160"/>
+    <mergeCell ref="Q161:V161"/>
+    <mergeCell ref="Q162:V162"/>
+    <mergeCell ref="Q139:V139"/>
+    <mergeCell ref="Q140:V140"/>
+    <mergeCell ref="Q141:V141"/>
+    <mergeCell ref="Q142:V142"/>
+    <mergeCell ref="Q143:V143"/>
+    <mergeCell ref="Q144:V144"/>
+    <mergeCell ref="Q145:V145"/>
+    <mergeCell ref="Q146:V146"/>
+    <mergeCell ref="Q129:V129"/>
+    <mergeCell ref="Q137:V137"/>
+    <mergeCell ref="Q138:V138"/>
+    <mergeCell ref="Q130:V130"/>
+    <mergeCell ref="Q131:V131"/>
+    <mergeCell ref="Q132:V132"/>
+    <mergeCell ref="Q133:V133"/>
+    <mergeCell ref="Q134:V134"/>
+    <mergeCell ref="Q135:V135"/>
+    <mergeCell ref="Q136:V136"/>
+    <mergeCell ref="Q121:V121"/>
+    <mergeCell ref="Q122:V122"/>
+    <mergeCell ref="Q123:V123"/>
+    <mergeCell ref="Q124:V124"/>
+    <mergeCell ref="Q125:V125"/>
+    <mergeCell ref="Q126:V126"/>
+    <mergeCell ref="Q127:V127"/>
+    <mergeCell ref="Q128:V128"/>
+    <mergeCell ref="Q110:V110"/>
+    <mergeCell ref="Q111:V111"/>
+    <mergeCell ref="Q112:V112"/>
+    <mergeCell ref="Q113:V113"/>
+    <mergeCell ref="Q114:V114"/>
+    <mergeCell ref="Q115:V115"/>
+    <mergeCell ref="Q116:V116"/>
+    <mergeCell ref="Q117:V117"/>
+    <mergeCell ref="Q118:V118"/>
+    <mergeCell ref="Q119:V119"/>
+    <mergeCell ref="Q120:V120"/>
+    <mergeCell ref="Q108:V108"/>
+    <mergeCell ref="Q53:V53"/>
+    <mergeCell ref="Q54:V54"/>
+    <mergeCell ref="Q32:V32"/>
+    <mergeCell ref="Q33:V33"/>
+    <mergeCell ref="Q34:V34"/>
+    <mergeCell ref="Q35:V35"/>
+    <mergeCell ref="Q26:V26"/>
+    <mergeCell ref="Q27:V27"/>
+    <mergeCell ref="Q28:V28"/>
+    <mergeCell ref="Q29:V29"/>
+    <mergeCell ref="Q30:V30"/>
+    <mergeCell ref="Q61:V61"/>
+    <mergeCell ref="Q62:V62"/>
+    <mergeCell ref="Q63:V63"/>
+    <mergeCell ref="Q64:V64"/>
+    <mergeCell ref="Q41:V41"/>
+    <mergeCell ref="Q42:V42"/>
+    <mergeCell ref="Q43:V43"/>
+    <mergeCell ref="Q44:V44"/>
+    <mergeCell ref="Q45:V45"/>
+    <mergeCell ref="Q36:V36"/>
+    <mergeCell ref="Q37:V37"/>
+    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="Q50:V50"/>
+    <mergeCell ref="Q51:V51"/>
+    <mergeCell ref="Q52:V52"/>
+    <mergeCell ref="Q46:V46"/>
+    <mergeCell ref="Q14:V14"/>
+    <mergeCell ref="Q15:V15"/>
+    <mergeCell ref="Q16:V16"/>
+    <mergeCell ref="Q17:V17"/>
+    <mergeCell ref="Q47:V47"/>
+    <mergeCell ref="Q48:V48"/>
+    <mergeCell ref="Q49:V49"/>
+    <mergeCell ref="Q39:V39"/>
+    <mergeCell ref="Q40:V40"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H6"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="Q109:V109"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="Q8:V8"/>
+    <mergeCell ref="Q10:V10"/>
+    <mergeCell ref="Q11:V11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="Q19:V19"/>
+    <mergeCell ref="Q20:V20"/>
+    <mergeCell ref="Q12:V12"/>
+    <mergeCell ref="Q13:V13"/>
+    <mergeCell ref="Q31:V31"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="Q25:V25"/>
+    <mergeCell ref="Q24:V24"/>
+    <mergeCell ref="Q22:V22"/>
+    <mergeCell ref="Q23:V23"/>
+    <mergeCell ref="Q55:V55"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="Q18:V18"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="Q21:V21"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="Q5:V5"/>
+    <mergeCell ref="Q6:V6"/>
+    <mergeCell ref="Q7:V7"/>
+    <mergeCell ref="Q72:V72"/>
+    <mergeCell ref="Q73:V73"/>
+    <mergeCell ref="C37:D38"/>
+    <mergeCell ref="E37:F38"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="H8:L9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="Q84:V84"/>
+    <mergeCell ref="Q85:V85"/>
+    <mergeCell ref="Q76:V76"/>
+    <mergeCell ref="Q77:V77"/>
+    <mergeCell ref="Q78:V78"/>
+    <mergeCell ref="Q79:V79"/>
+    <mergeCell ref="Q80:V80"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="Q74:V74"/>
+    <mergeCell ref="Q75:V75"/>
+    <mergeCell ref="Q66:V66"/>
+    <mergeCell ref="Q67:V67"/>
+    <mergeCell ref="Q68:V68"/>
+    <mergeCell ref="Q69:V69"/>
+    <mergeCell ref="Q70:V70"/>
+    <mergeCell ref="Q81:V81"/>
+    <mergeCell ref="Q82:V82"/>
+    <mergeCell ref="Q65:V65"/>
+    <mergeCell ref="Q56:V56"/>
+    <mergeCell ref="Q57:V57"/>
+    <mergeCell ref="Q58:V58"/>
+    <mergeCell ref="Q59:V59"/>
+    <mergeCell ref="Q60:V60"/>
+    <mergeCell ref="Q71:V71"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="Q106:V106"/>
     <mergeCell ref="Q107:V107"/>
@@ -6894,234 +7101,27 @@
     <mergeCell ref="Q89:V89"/>
     <mergeCell ref="Q90:V90"/>
     <mergeCell ref="Q83:V83"/>
-    <mergeCell ref="Q84:V84"/>
-    <mergeCell ref="Q85:V85"/>
-    <mergeCell ref="Q76:V76"/>
-    <mergeCell ref="Q77:V77"/>
-    <mergeCell ref="Q78:V78"/>
-    <mergeCell ref="Q79:V79"/>
-    <mergeCell ref="Q80:V80"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="Q74:V74"/>
-    <mergeCell ref="Q75:V75"/>
-    <mergeCell ref="Q66:V66"/>
-    <mergeCell ref="Q67:V67"/>
-    <mergeCell ref="Q68:V68"/>
-    <mergeCell ref="Q69:V69"/>
-    <mergeCell ref="Q70:V70"/>
-    <mergeCell ref="Q81:V81"/>
-    <mergeCell ref="Q82:V82"/>
-    <mergeCell ref="Q65:V65"/>
-    <mergeCell ref="Q56:V56"/>
-    <mergeCell ref="Q57:V57"/>
-    <mergeCell ref="Q58:V58"/>
-    <mergeCell ref="Q59:V59"/>
-    <mergeCell ref="Q60:V60"/>
-    <mergeCell ref="Q71:V71"/>
-    <mergeCell ref="Q72:V72"/>
-    <mergeCell ref="Q73:V73"/>
-    <mergeCell ref="C37:D38"/>
-    <mergeCell ref="E37:F38"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="H8:L9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="Q18:V18"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="Q21:V21"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H6"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="Q109:V109"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="Q8:V8"/>
-    <mergeCell ref="Q10:V10"/>
-    <mergeCell ref="Q11:V11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="Q19:V19"/>
-    <mergeCell ref="Q20:V20"/>
-    <mergeCell ref="Q12:V12"/>
-    <mergeCell ref="Q13:V13"/>
-    <mergeCell ref="Q31:V31"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="Q25:V25"/>
-    <mergeCell ref="Q24:V24"/>
-    <mergeCell ref="Q22:V22"/>
-    <mergeCell ref="Q23:V23"/>
-    <mergeCell ref="Q55:V55"/>
-    <mergeCell ref="Q50:V50"/>
-    <mergeCell ref="Q51:V51"/>
-    <mergeCell ref="Q52:V52"/>
-    <mergeCell ref="Q46:V46"/>
-    <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="Q16:V16"/>
-    <mergeCell ref="Q17:V17"/>
-    <mergeCell ref="Q47:V47"/>
-    <mergeCell ref="Q48:V48"/>
-    <mergeCell ref="Q49:V49"/>
-    <mergeCell ref="Q108:V108"/>
-    <mergeCell ref="Q53:V53"/>
-    <mergeCell ref="Q54:V54"/>
-    <mergeCell ref="Q32:V32"/>
-    <mergeCell ref="Q33:V33"/>
-    <mergeCell ref="Q34:V34"/>
-    <mergeCell ref="Q35:V35"/>
-    <mergeCell ref="Q26:V26"/>
-    <mergeCell ref="Q27:V27"/>
-    <mergeCell ref="Q28:V28"/>
-    <mergeCell ref="Q29:V29"/>
-    <mergeCell ref="Q30:V30"/>
-    <mergeCell ref="Q61:V61"/>
-    <mergeCell ref="Q62:V62"/>
-    <mergeCell ref="Q63:V63"/>
-    <mergeCell ref="Q64:V64"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="Q5:V5"/>
-    <mergeCell ref="Q6:V6"/>
-    <mergeCell ref="Q7:V7"/>
-    <mergeCell ref="Q41:V41"/>
-    <mergeCell ref="Q42:V42"/>
-    <mergeCell ref="Q43:V43"/>
-    <mergeCell ref="Q44:V44"/>
-    <mergeCell ref="Q45:V45"/>
-    <mergeCell ref="Q36:V36"/>
-    <mergeCell ref="Q37:V37"/>
-    <mergeCell ref="Q38:V38"/>
-    <mergeCell ref="Q39:V39"/>
-    <mergeCell ref="Q40:V40"/>
-    <mergeCell ref="Q121:V121"/>
-    <mergeCell ref="Q122:V122"/>
-    <mergeCell ref="Q123:V123"/>
-    <mergeCell ref="Q124:V124"/>
-    <mergeCell ref="Q125:V125"/>
-    <mergeCell ref="Q126:V126"/>
-    <mergeCell ref="Q127:V127"/>
-    <mergeCell ref="Q128:V128"/>
-    <mergeCell ref="Q110:V110"/>
-    <mergeCell ref="Q111:V111"/>
-    <mergeCell ref="Q112:V112"/>
-    <mergeCell ref="Q113:V113"/>
-    <mergeCell ref="Q114:V114"/>
-    <mergeCell ref="Q115:V115"/>
-    <mergeCell ref="Q116:V116"/>
-    <mergeCell ref="Q117:V117"/>
-    <mergeCell ref="Q118:V118"/>
-    <mergeCell ref="Q119:V119"/>
-    <mergeCell ref="Q120:V120"/>
-    <mergeCell ref="Q139:V139"/>
-    <mergeCell ref="Q140:V140"/>
-    <mergeCell ref="Q141:V141"/>
-    <mergeCell ref="Q142:V142"/>
-    <mergeCell ref="Q143:V143"/>
-    <mergeCell ref="Q144:V144"/>
-    <mergeCell ref="Q145:V145"/>
-    <mergeCell ref="Q146:V146"/>
-    <mergeCell ref="Q129:V129"/>
-    <mergeCell ref="Q137:V137"/>
-    <mergeCell ref="Q138:V138"/>
-    <mergeCell ref="Q130:V130"/>
-    <mergeCell ref="Q131:V131"/>
-    <mergeCell ref="Q132:V132"/>
-    <mergeCell ref="Q133:V133"/>
-    <mergeCell ref="Q134:V134"/>
-    <mergeCell ref="Q135:V135"/>
-    <mergeCell ref="Q136:V136"/>
-    <mergeCell ref="Q164:V164"/>
-    <mergeCell ref="Q147:V147"/>
-    <mergeCell ref="Q155:V155"/>
-    <mergeCell ref="Q156:V156"/>
-    <mergeCell ref="Q148:V148"/>
-    <mergeCell ref="Q149:V149"/>
-    <mergeCell ref="Q150:V150"/>
-    <mergeCell ref="Q151:V151"/>
-    <mergeCell ref="Q152:V152"/>
-    <mergeCell ref="Q153:V153"/>
-    <mergeCell ref="Q154:V154"/>
-    <mergeCell ref="Q163:V163"/>
-    <mergeCell ref="Q157:V157"/>
-    <mergeCell ref="Q158:V158"/>
-    <mergeCell ref="Q159:V159"/>
-    <mergeCell ref="Q160:V160"/>
-    <mergeCell ref="Q161:V161"/>
-    <mergeCell ref="Q162:V162"/>
-    <mergeCell ref="Q210:V210"/>
-    <mergeCell ref="Q198:V198"/>
-    <mergeCell ref="Q199:V199"/>
-    <mergeCell ref="Q200:V200"/>
-    <mergeCell ref="Q201:V201"/>
-    <mergeCell ref="Q202:V202"/>
-    <mergeCell ref="Q203:V203"/>
-    <mergeCell ref="Q204:V204"/>
-    <mergeCell ref="Q205:V205"/>
-    <mergeCell ref="Q206:V206"/>
-    <mergeCell ref="Q165:V165"/>
-    <mergeCell ref="Q182:V182"/>
-    <mergeCell ref="Q190:V190"/>
-    <mergeCell ref="Q167:V167"/>
-    <mergeCell ref="Q168:V168"/>
-    <mergeCell ref="Q169:V169"/>
-    <mergeCell ref="Q170:V170"/>
-    <mergeCell ref="Q171:V171"/>
-    <mergeCell ref="Q172:V172"/>
-    <mergeCell ref="Q173:V173"/>
-    <mergeCell ref="Q189:V189"/>
-    <mergeCell ref="Q183:V183"/>
-    <mergeCell ref="Q184:V184"/>
-    <mergeCell ref="Q185:V185"/>
-    <mergeCell ref="Q186:V186"/>
-    <mergeCell ref="Q187:V187"/>
-    <mergeCell ref="Q188:V188"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="Q207:V207"/>
-    <mergeCell ref="Q208:V208"/>
-    <mergeCell ref="Q209:V209"/>
-    <mergeCell ref="Q175:V175"/>
-    <mergeCell ref="Q176:V176"/>
-    <mergeCell ref="Q177:V177"/>
-    <mergeCell ref="Q178:V178"/>
-    <mergeCell ref="Q179:V179"/>
-    <mergeCell ref="Q197:V197"/>
-    <mergeCell ref="Q180:V180"/>
-    <mergeCell ref="Q181:V181"/>
-    <mergeCell ref="Q191:V191"/>
-    <mergeCell ref="Q192:V192"/>
-    <mergeCell ref="Q193:V193"/>
-    <mergeCell ref="Q194:V194"/>
-    <mergeCell ref="Q195:V195"/>
-    <mergeCell ref="Q196:V196"/>
-    <mergeCell ref="Q166:V166"/>
-    <mergeCell ref="Q174:V174"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="360" r:id="rId1"/>
@@ -7135,7 +7135,7 @@
   <dimension ref="A1:BT326"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M4"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7247,22 +7247,22 @@
         <v>5</v>
       </c>
       <c r="N2" s="53"/>
-      <c r="O2" s="285" t="s">
+      <c r="O2" s="342" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="291" t="s">
+      <c r="P2" s="343"/>
+      <c r="Q2" s="344"/>
+      <c r="R2" s="348" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="310" t="s">
+      <c r="S2" s="334" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="53"/>
       <c r="U2" s="53"/>
       <c r="V2" s="53"/>
-      <c r="W2" s="303"/>
-      <c r="X2" s="303"/>
+      <c r="W2" s="327"/>
+      <c r="X2" s="327"/>
       <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
@@ -7297,31 +7297,31 @@
     <row r="3" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="294">
+      <c r="C3" s="351">
         <f>НалБанки!C3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="280">
+      <c r="D3" s="337">
         <f>НалБанки!D3</f>
         <v>0</v>
       </c>
-      <c r="E3" s="280">
+      <c r="E3" s="337">
         <f>НалБанки!E3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="280">
+      <c r="F3" s="337">
         <f>НалБанки!F3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="280">
+      <c r="G3" s="337">
         <f>НалБанки!G3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="280">
+      <c r="H3" s="337">
         <f>НалБанки!H3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="282">
+      <c r="I3" s="339">
         <f>НалБанки!I3</f>
         <v>40</v>
       </c>
@@ -7333,25 +7333,25 @@
         <f>ROUNDUP(((SUM(D3:F4,H3:I4)+(SUM(G3:G4)*0.75))*L3+((SUM(D3:F4,I3)+SUM(G3:G4)*0.75)*20%+(SUM(D3:F4,H3:I4)+SUM(G3:G4)*0.75)))*M3,0)</f>
         <v>167</v>
       </c>
-      <c r="L3" s="304">
+      <c r="L3" s="328">
         <f>8/92*1.2</f>
         <v>0.10434782608695652</v>
       </c>
-      <c r="M3" s="306">
+      <c r="M3" s="330">
         <f>НалБанки!J3</f>
         <v>3.2</v>
       </c>
       <c r="N3" s="53"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="289"/>
-      <c r="Q3" s="290"/>
-      <c r="R3" s="292"/>
-      <c r="S3" s="311"/>
+      <c r="O3" s="345"/>
+      <c r="P3" s="346"/>
+      <c r="Q3" s="347"/>
+      <c r="R3" s="349"/>
+      <c r="S3" s="335"/>
       <c r="T3" s="53"/>
       <c r="U3" s="53"/>
       <c r="V3" s="53"/>
-      <c r="W3" s="303"/>
-      <c r="X3" s="303"/>
+      <c r="W3" s="327"/>
+      <c r="X3" s="327"/>
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
@@ -7386,13 +7386,13 @@
     <row r="4" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="295"/>
-      <c r="D4" s="296"/>
-      <c r="E4" s="296"/>
-      <c r="F4" s="296"/>
-      <c r="G4" s="296"/>
-      <c r="H4" s="281"/>
-      <c r="I4" s="283"/>
+      <c r="C4" s="352"/>
+      <c r="D4" s="353"/>
+      <c r="E4" s="353"/>
+      <c r="F4" s="353"/>
+      <c r="G4" s="353"/>
+      <c r="H4" s="338"/>
+      <c r="I4" s="340"/>
       <c r="J4" s="50">
         <f>J3-(J3-H3*M3)/6</f>
         <v>139.16666666666666</v>
@@ -7401,8 +7401,8 @@
         <f>K3-(K3-H3*M3)/6</f>
         <v>139.16666666666666</v>
       </c>
-      <c r="L4" s="305"/>
-      <c r="M4" s="307"/>
+      <c r="L4" s="329"/>
+      <c r="M4" s="331"/>
       <c r="N4" s="53"/>
       <c r="O4" s="15" t="s">
         <v>7</v>
@@ -7413,8 +7413,8 @@
       <c r="Q4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="293"/>
-      <c r="S4" s="312"/>
+      <c r="R4" s="350"/>
+      <c r="S4" s="336"/>
       <c r="T4" s="53"/>
       <c r="U4" s="53"/>
       <c r="V4" s="62" t="s">
@@ -7456,15 +7456,15 @@
     <row r="5" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="297">
+      <c r="C5" s="354">
         <f ca="1">TODAY()</f>
-        <v>45364</v>
-      </c>
-      <c r="D5" s="298"/>
-      <c r="E5" s="298"/>
-      <c r="F5" s="298"/>
-      <c r="G5" s="298"/>
-      <c r="H5" s="298"/>
+        <v>45490</v>
+      </c>
+      <c r="D5" s="355"/>
+      <c r="E5" s="355"/>
+      <c r="F5" s="355"/>
+      <c r="G5" s="355"/>
+      <c r="H5" s="355"/>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
@@ -7475,20 +7475,20 @@
         <v>19</v>
       </c>
       <c r="P5" s="18">
-        <f>ROUNDUP($J$3/100*(100+V5),0)</f>
-        <v>239</v>
+        <f>ROUNDUP($J$3/100*(100+V5),-1)</f>
+        <v>240</v>
       </c>
       <c r="Q5" s="18">
-        <f>ROUNDUP($K$3/100*(100+V5),0)</f>
-        <v>239</v>
+        <f>ROUNDUP($K$3/100*(100+V5),-1)</f>
+        <v>240</v>
       </c>
       <c r="R5" s="19">
         <f>P5/4</f>
-        <v>59.75</v>
+        <v>60</v>
       </c>
       <c r="S5" s="20">
         <f>Q5/4</f>
-        <v>59.75</v>
+        <v>60</v>
       </c>
       <c r="T5" s="53"/>
       <c r="U5" s="53"/>
@@ -7531,10 +7531,10 @@
     <row r="6" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
+      <c r="C6" s="341"/>
+      <c r="D6" s="341"/>
+      <c r="E6" s="341"/>
+      <c r="F6" s="341"/>
       <c r="G6" s="9"/>
       <c r="H6" s="29"/>
       <c r="I6" s="10"/>
@@ -7547,20 +7547,20 @@
         <v>9</v>
       </c>
       <c r="P6" s="18">
-        <f t="shared" ref="P6:P9" si="0">ROUNDUP($J$3/100*(100+V6),0)</f>
-        <v>248</v>
+        <f>ROUNDUP($J$3/100*(100+V6),-1)</f>
+        <v>250</v>
       </c>
       <c r="Q6" s="18">
-        <f t="shared" ref="Q6:Q9" si="1">ROUNDUP($K$3/100*(100+V6),0)</f>
-        <v>248</v>
+        <f>ROUNDUP($K$3/100*(100+V6),-1)</f>
+        <v>250</v>
       </c>
       <c r="R6" s="22">
         <f>P6/6</f>
-        <v>41.333333333333336</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="S6" s="23">
         <f>Q6/6</f>
-        <v>41.333333333333336</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="T6" s="53"/>
       <c r="U6" s="53"/>
@@ -7619,20 +7619,20 @@
         <v>10</v>
       </c>
       <c r="P7" s="18">
-        <f t="shared" si="0"/>
-        <v>272</v>
+        <f>ROUNDUP($J$3/100*(100+V7),-1)</f>
+        <v>280</v>
       </c>
       <c r="Q7" s="18">
-        <f t="shared" si="1"/>
-        <v>272</v>
+        <f>ROUNDUP($K$3/100*(100+V7),-1)</f>
+        <v>280</v>
       </c>
       <c r="R7" s="22">
         <f>P7/12</f>
-        <v>22.666666666666668</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="S7" s="23">
         <f>Q7/12</f>
-        <v>22.666666666666668</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="T7" s="53"/>
       <c r="U7" s="53"/>
@@ -7675,17 +7675,17 @@
     <row r="8" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="313" t="s">
+      <c r="C8" s="299" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="314"/>
-      <c r="E8" s="315"/>
+      <c r="D8" s="300"/>
+      <c r="E8" s="301"/>
       <c r="F8" s="34"/>
-      <c r="G8" s="319" t="s">
+      <c r="G8" s="305" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="320"/>
-      <c r="I8" s="321"/>
+      <c r="H8" s="306"/>
+      <c r="I8" s="307"/>
       <c r="J8" s="54"/>
       <c r="K8" s="55"/>
       <c r="L8" s="55"/>
@@ -7695,20 +7695,20 @@
         <v>20</v>
       </c>
       <c r="P8" s="18">
-        <f t="shared" si="0"/>
-        <v>322</v>
+        <f>ROUNDUP($J$3/100*(100+V8),-1)</f>
+        <v>330</v>
       </c>
       <c r="Q8" s="18">
-        <f t="shared" si="1"/>
-        <v>322</v>
+        <f>ROUNDUP($K$3/100*(100+V8),-1)</f>
+        <v>330</v>
       </c>
       <c r="R8" s="22">
         <f>P8/20</f>
-        <v>16.100000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="S8" s="23">
         <f>Q8/20</f>
-        <v>16.100000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="T8" s="53"/>
       <c r="U8" s="53"/>
@@ -7751,13 +7751,13 @@
     <row r="9" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="316"/>
-      <c r="D9" s="317"/>
-      <c r="E9" s="318"/>
+      <c r="C9" s="302"/>
+      <c r="D9" s="303"/>
+      <c r="E9" s="304"/>
       <c r="F9" s="35"/>
-      <c r="G9" s="322"/>
-      <c r="H9" s="323"/>
-      <c r="I9" s="324"/>
+      <c r="G9" s="308"/>
+      <c r="H9" s="309"/>
+      <c r="I9" s="310"/>
       <c r="J9" s="54"/>
       <c r="K9" s="55"/>
       <c r="L9" s="55"/>
@@ -7767,20 +7767,20 @@
         <v>12</v>
       </c>
       <c r="P9" s="18">
-        <f t="shared" si="0"/>
-        <v>329</v>
+        <f>ROUNDUP($J$3/100*(100+V9),-1)</f>
+        <v>330</v>
       </c>
       <c r="Q9" s="18">
-        <f t="shared" si="1"/>
-        <v>329</v>
+        <f>ROUNDUP($K$3/100*(100+V9),-1)</f>
+        <v>330</v>
       </c>
       <c r="R9" s="25">
         <f>P9/24</f>
-        <v>13.708333333333334</v>
+        <v>13.75</v>
       </c>
       <c r="S9" s="26">
         <f>Q9/24</f>
-        <v>13.708333333333334</v>
+        <v>13.75</v>
       </c>
       <c r="T9" s="53"/>
       <c r="U9" s="53"/>
@@ -7823,23 +7823,23 @@
     <row r="10" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="325" t="s">
+      <c r="C10" s="311" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="327" t="s">
+      <c r="D10" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="329" t="s">
+      <c r="E10" s="315" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="37"/>
-      <c r="G10" s="331" t="s">
+      <c r="G10" s="317" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="333" t="s">
+      <c r="H10" s="319" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="335" t="s">
+      <c r="I10" s="321" t="s">
         <v>14</v>
       </c>
       <c r="J10" s="54"/>
@@ -7891,13 +7891,13 @@
     <row r="11" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="326"/>
-      <c r="D11" s="328"/>
-      <c r="E11" s="330"/>
+      <c r="C11" s="312"/>
+      <c r="D11" s="314"/>
+      <c r="E11" s="316"/>
       <c r="F11" s="31"/>
-      <c r="G11" s="332"/>
-      <c r="H11" s="334"/>
-      <c r="I11" s="336"/>
+      <c r="G11" s="318"/>
+      <c r="H11" s="320"/>
+      <c r="I11" s="322"/>
       <c r="J11" s="54"/>
       <c r="K11" s="55"/>
       <c r="L11" s="55"/>
@@ -7951,12 +7951,12 @@
         <v>19</v>
       </c>
       <c r="D12" s="39">
-        <f t="shared" ref="D12:E16" si="2">P5*0.03</f>
-        <v>7.17</v>
+        <f t="shared" ref="D12:E16" si="0">P5*0.03</f>
+        <v>7.1999999999999993</v>
       </c>
       <c r="E12" s="40">
-        <f t="shared" si="2"/>
-        <v>7.17</v>
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="38" t="s">
@@ -7964,11 +7964,11 @@
       </c>
       <c r="H12" s="41">
         <f>(P5-(SUM(H3:H4)*M3))/6</f>
-        <v>39.833333333333336</v>
+        <v>40</v>
       </c>
       <c r="I12" s="42">
         <f>(Q5-(SUM(H3:H4)*M3))/6</f>
-        <v>39.833333333333336</v>
+        <v>40</v>
       </c>
       <c r="J12" s="54"/>
       <c r="K12" s="55"/>
@@ -7977,14 +7977,14 @@
       <c r="N12" s="53"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
-      <c r="R12" s="299" t="s">
+      <c r="R12" s="323" t="s">
         <v>21</v>
       </c>
-      <c r="S12" s="300"/>
-      <c r="T12" s="308" t="s">
+      <c r="S12" s="324"/>
+      <c r="T12" s="332" t="s">
         <v>30</v>
       </c>
-      <c r="U12" s="309"/>
+      <c r="U12" s="333"/>
       <c r="V12" s="53"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
@@ -8026,12 +8026,12 @@
         <v>9</v>
       </c>
       <c r="D13" s="39">
-        <f t="shared" si="2"/>
-        <v>7.4399999999999995</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="E13" s="40">
-        <f t="shared" si="2"/>
-        <v>7.4399999999999995</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="21" t="s">
@@ -8039,11 +8039,11 @@
       </c>
       <c r="H13" s="41">
         <f>(P6-(SUM(H3:H4)*M3))/6</f>
-        <v>41.333333333333336</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="I13" s="42">
         <f>(Q6-(SUM(H3:H4)*M3))/6</f>
-        <v>41.333333333333336</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="J13" s="54"/>
       <c r="K13" s="55"/>
@@ -8052,8 +8052,8 @@
       <c r="N13" s="53"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
-      <c r="R13" s="301"/>
-      <c r="S13" s="302"/>
+      <c r="R13" s="325"/>
+      <c r="S13" s="326"/>
       <c r="T13" s="56" t="s">
         <v>21</v>
       </c>
@@ -8101,12 +8101,12 @@
         <v>10</v>
       </c>
       <c r="D14" s="39">
-        <f t="shared" si="2"/>
-        <v>8.16</v>
+        <f t="shared" si="0"/>
+        <v>8.4</v>
       </c>
       <c r="E14" s="40">
-        <f t="shared" si="2"/>
-        <v>8.16</v>
+        <f t="shared" si="0"/>
+        <v>8.4</v>
       </c>
       <c r="F14" s="36"/>
       <c r="G14" s="21" t="s">
@@ -8114,34 +8114,34 @@
       </c>
       <c r="H14" s="41">
         <f>(P7-(SUM(H3:H4)*M3))/6</f>
-        <v>45.333333333333336</v>
+        <v>46.666666666666664</v>
       </c>
       <c r="I14" s="42">
         <f>(Q7-(SUM(H3:H4)*M3))/6</f>
-        <v>45.333333333333336</v>
+        <v>46.666666666666664</v>
       </c>
       <c r="J14" s="54"/>
       <c r="K14" s="55"/>
       <c r="L14" s="55"/>
       <c r="M14" s="55"/>
       <c r="N14" s="53"/>
-      <c r="O14" s="343" t="s">
+      <c r="O14" s="287" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="344"/>
-      <c r="Q14" s="347">
+      <c r="P14" s="288"/>
+      <c r="Q14" s="291">
         <v>0.02</v>
       </c>
-      <c r="R14" s="353">
+      <c r="R14" s="297">
         <f>IF(R12="ЖЕЛ",J4*Q14,K4*Q14)</f>
         <v>2.7833333333333332</v>
       </c>
-      <c r="S14" s="354"/>
-      <c r="T14" s="337">
+      <c r="S14" s="298"/>
+      <c r="T14" s="281">
         <f>J4</f>
         <v>139.16666666666666</v>
       </c>
-      <c r="U14" s="340">
+      <c r="U14" s="284">
         <f>K4</f>
         <v>139.16666666666666</v>
       </c>
@@ -8186,12 +8186,12 @@
         <v>20</v>
       </c>
       <c r="D15" s="39">
-        <f t="shared" si="2"/>
-        <v>9.66</v>
+        <f t="shared" si="0"/>
+        <v>9.9</v>
       </c>
       <c r="E15" s="40">
-        <f t="shared" si="2"/>
-        <v>9.66</v>
+        <f t="shared" si="0"/>
+        <v>9.9</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="21" t="s">
@@ -8199,24 +8199,24 @@
       </c>
       <c r="H15" s="41">
         <f>(P8-(SUM(H3:H4)*M3))/6</f>
-        <v>53.666666666666664</v>
+        <v>55</v>
       </c>
       <c r="I15" s="42">
         <f>(Q8-(SUM(H3:H4)*M3))/6</f>
-        <v>53.666666666666664</v>
+        <v>55</v>
       </c>
       <c r="J15" s="54"/>
       <c r="K15" s="55"/>
       <c r="L15" s="55"/>
       <c r="M15" s="55"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="345"/>
-      <c r="P15" s="346"/>
-      <c r="Q15" s="348"/>
-      <c r="R15" s="351"/>
-      <c r="S15" s="352"/>
-      <c r="T15" s="338"/>
-      <c r="U15" s="341"/>
+      <c r="O15" s="289"/>
+      <c r="P15" s="290"/>
+      <c r="Q15" s="292"/>
+      <c r="R15" s="295"/>
+      <c r="S15" s="296"/>
+      <c r="T15" s="282"/>
+      <c r="U15" s="285"/>
       <c r="V15" s="9"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
@@ -8258,12 +8258,12 @@
         <v>12</v>
       </c>
       <c r="D16" s="44">
-        <f t="shared" si="2"/>
-        <v>9.8699999999999992</v>
+        <f t="shared" si="0"/>
+        <v>9.9</v>
       </c>
       <c r="E16" s="45">
-        <f t="shared" si="2"/>
-        <v>9.8699999999999992</v>
+        <f t="shared" si="0"/>
+        <v>9.9</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="24" t="s">
@@ -8271,31 +8271,31 @@
       </c>
       <c r="H16" s="46">
         <f>(P9-(SUM(H3:H4)*M3))/6</f>
-        <v>54.833333333333336</v>
+        <v>55</v>
       </c>
       <c r="I16" s="47">
         <f>(Q9-(SUM(H3:H4)*M3))/6</f>
-        <v>54.833333333333336</v>
+        <v>55</v>
       </c>
       <c r="J16" s="54"/>
       <c r="K16" s="55"/>
       <c r="L16" s="55"/>
       <c r="M16" s="55"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="343" t="s">
+      <c r="O16" s="287" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="344"/>
-      <c r="Q16" s="347">
+      <c r="P16" s="288"/>
+      <c r="Q16" s="291">
         <v>0</v>
       </c>
-      <c r="R16" s="349">
+      <c r="R16" s="293">
         <f>IF(R12="ЖЕЛ",J4*Q16,K4*Q16)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="350"/>
-      <c r="T16" s="338"/>
-      <c r="U16" s="341"/>
+      <c r="S16" s="294"/>
+      <c r="T16" s="282"/>
+      <c r="U16" s="285"/>
       <c r="V16" s="9"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
@@ -8345,13 +8345,13 @@
       <c r="L17" s="43"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="345"/>
-      <c r="P17" s="346"/>
-      <c r="Q17" s="348"/>
-      <c r="R17" s="351"/>
-      <c r="S17" s="352"/>
-      <c r="T17" s="339"/>
-      <c r="U17" s="342"/>
+      <c r="O17" s="289"/>
+      <c r="P17" s="290"/>
+      <c r="Q17" s="292"/>
+      <c r="R17" s="295"/>
+      <c r="S17" s="296"/>
+      <c r="T17" s="283"/>
+      <c r="U17" s="286"/>
       <c r="V17" s="9"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
@@ -15472,29 +15472,6 @@
     <protectedRange sqref="L3:L4 J3:K3" name="Диапазон1_1_2_1_1"/>
   </protectedRanges>
   <mergeCells count="34">
-    <mergeCell ref="T14:T17"/>
-    <mergeCell ref="U14:U17"/>
-    <mergeCell ref="O16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:S17"/>
-    <mergeCell ref="O14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:S15"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="G8:I9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="R12:S13"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="S2:S4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="C6:F6"/>
@@ -15506,6 +15483,29 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="C5:H5"/>
+    <mergeCell ref="R12:S13"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="G8:I9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="T14:T17"/>
+    <mergeCell ref="U14:U17"/>
+    <mergeCell ref="O16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:S17"/>
+    <mergeCell ref="O14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:S15"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R12">

</xml_diff>